<commit_message>
Updates to country project output
</commit_message>
<xml_diff>
--- a/Inputs/FCDO core contribution programmes (with beneficiary countries).xlsx
+++ b/Inputs/FCDO core contribution programmes (with beneficiary countries).xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wellcomecloud-my.sharepoint.com/personal/e_clegg_ukcds_org_uk/Documents/My Documents/GitHub/ODA_research_and_innovation/Inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e-clegg\Documents\GitHub projects\ODA_research_and_innovation\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="165" documentId="13_ncr:1_{AA5B4C96-D9A2-4DF5-AD3E-B21AF2628C12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{45A4A303-0AF2-47EE-BE3F-DBE8EDA44EEC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070E39C3-B5FA-4896-9E25-FB4E27AA2A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FCDO core contribution projects" sheetId="4" r:id="rId1"/>
     <sheet name="RED geotagging (from AMP)" sheetId="6" r:id="rId2"/>
+    <sheet name="RED geotagging (from AMP) (2)" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FCDO core contribution projects'!$A$1:$C$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FCDO core contribution projects'!$A$1:$C$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'RED geotagging (from AMP)'!$A$1:$I$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'RED geotagging (from AMP) (2)'!$A$1:$L$92</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="408">
   <si>
     <t>KENYA,MOZAMBIQUE,PAKISTAN,SIERRA LEONE,TUVALU</t>
   </si>
@@ -1076,6 +1078,189 @@
   </si>
   <si>
     <t>GB-1-203052-104</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>This Programme Supports A Global Public Good</t>
+  </si>
+  <si>
+    <t>This Programme Supports A Regional Public Good</t>
+  </si>
+  <si>
+    <t>Kenya,Tanzania,Ghana,Nigeria,Rwanda,South Africa</t>
+  </si>
+  <si>
+    <t>Kenya,Uganda,Ethiopia,Bangladesh,Mozambique,Malawi,Pakistan</t>
+  </si>
+  <si>
+    <t>Kenya,Uganda,Tanzania,Nigeria,Zambia,Senegal,Viet Nam,Indonesia</t>
+  </si>
+  <si>
+    <t>Kenya,Uganda,Ethiopia,Bangladesh,Ghana,Nigeria,Mozambique,Rwanda,Pakistan,Sierra Leone,Nepal,India,Afghanistan,Bhutan,Kyrgyzstan</t>
+  </si>
+  <si>
+    <t>Kenya,Mozambique,Pakistan,Sierra Leone,Tuvalu</t>
+  </si>
+  <si>
+    <t>Kenya,Uganda,Tanzania,Ethiopia,Ghana,Nigeria,Mozambique,Zambia,Malawi,Zimbabwe,Drc,South Africa</t>
+  </si>
+  <si>
+    <t>Kenya,Uganda,Tanzania,Ethiopia,Bangladesh,Ghana,Nigeria,Zambia,Malawi,Rwanda,Pakistan,Sierra Leone,Nepal,Zimbabwe,Drc,Afghanistan,South Sudan,Senegal,Somalia,Sudan (The),Mali,Niger (The),Benin,Burkina Faso,Burundi,Cameroon,Chad,Côte D’Ivoire,Gambia (The),Jordan,Lebanon,Mauritania,Togo,Viet Nam</t>
+  </si>
+  <si>
+    <t>Nigeria,Pakistan,Afghanistan,South Sudan,Myanmar,Somalia,Sudan (The),Iran (Islamic Republic Of),Iraq,Syrian Arab Republic,Yemen,Egypt,Libyan Arab Jamahiriya,Chad,Tunisia,Algeria</t>
+  </si>
+  <si>
+    <t>Ethiopia,Bangladesh,Rwanda,Nepal,Jordan,Lebanon</t>
+  </si>
+  <si>
+    <t>Ethiopia,Bangladesh,Zambia,Malawi,Nepal</t>
+  </si>
+  <si>
+    <t>Tanzania,Ethiopia,Bangladesh,Nigeria,Mozambique,India,Myanmar,Madagascar</t>
+  </si>
+  <si>
+    <t>Kenya,Uganda,Ethiopia,Bangladesh,Nigeria</t>
+  </si>
+  <si>
+    <t>Kenya,Uganda,Tanzania,Ghana,Nigeria,Zambia,Malawi,Zimbabwe,Drc,South Africa,Senegal,Botswana,Burkina Faso,Cameroon,Gabon,Mauritius,Namibia,Congo (The)</t>
+  </si>
+  <si>
+    <t>Nigeria,South Sudan,Myanmar,Syrian Arab Republic,Jordan,Lebanon</t>
+  </si>
+  <si>
+    <t>Nigeria,Mozambique,Pakistan,Myanmar</t>
+  </si>
+  <si>
+    <t>Nigeria,Drc,South Sudan,Somalia</t>
+  </si>
+  <si>
+    <t>Kenya,Tanzania,Ethiopia,Ghana,Mozambique,Malawi,Zimbabwe</t>
+  </si>
+  <si>
+    <t>Kenya,Uganda,Ethiopia,Bangladesh,Ghana,Nigeria,Zambia,Rwanda,Pakistan,Nepal,India,Myanmar,Sudan (The),Egypt,Philippines (The)</t>
+  </si>
+  <si>
+    <t>Kenya,Tanzania,Ethiopia,Nigeria,Mozambique,Malawi,Rwanda,Pakistan,Nepal,India,South Africa,Senegal,Guinea-Bissau,Iraq,Liberia,Nicaragua,Tunisia</t>
+  </si>
+  <si>
+    <t>Kenya,Uganda,Tanzania,Ethiopia,Ghana,Nigeria,Mozambique,Zambia,Malawi,Rwanda,Sierra Leone,Drc,South Africa,South Sudan,Somalia,Niger (The),Côte D’Ivoire,Benin,Burkina Faso,Cameroon,Central African Republic (The),Guinea,Liberia,Madagascar,Mauritania,Congo (The),Togo</t>
+  </si>
+  <si>
+    <t>Kenya,Uganda,Nigeria,Malawi</t>
+  </si>
+  <si>
+    <t>Bangladesh,Pakistan,Nepal,India,Afghanistan,Myanmar</t>
+  </si>
+  <si>
+    <t>Ethiopia,Pakistan,Jamaica,Liberia</t>
+  </si>
+  <si>
+    <t>United Kingdom Of Great Britain And Northern Ireland (The)</t>
+  </si>
+  <si>
+    <t>Tanzania,Ethiopia,Nigeria,Pakistan,India,Indonesia,Viet Nam</t>
+  </si>
+  <si>
+    <t>Kenya,Uganda,Tanzania,Ethiopia,Bangladesh,Ghana,Nigeria,Mozambique,Malawi,Nepal,India,Niger (The),Burkina Faso,Guinea,Indonesia,Viet Nam</t>
+  </si>
+  <si>
+    <t>Kenya,Uganda,Tanzania,Ethiopia,Ghana,Nigeria,Zambia,Rwanda</t>
+  </si>
+  <si>
+    <t>Kenya,Uganda,Tanzania,Ethiopia,Ghana,Nigeria,Rwanda</t>
+  </si>
+  <si>
+    <t>Ethiopia,Drc,South Sudan,Sudan (The),Lebanon,Iraq,Syrian Arab Republic,Switzerland,Indonesia,United States Of America (The)</t>
+  </si>
+  <si>
+    <t>Kenya,Tanzania,Ghana,Nepal,Senegal,Côte D’Ivoire</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Nigeria,Malawi,Sierra Leone,South Sudan</t>
+  </si>
+  <si>
+    <t>This Is A Multi-Lateral Programme Which Is Core Funded</t>
+  </si>
+  <si>
+    <t>Kenya,Uganda,Tanzania,Ethiopia,Bangladesh,Ghana,Nigeria,Mozambique,Zambia,Malawi,Rwanda,Pakistan,Nepal,India,Drc,South Africa,Afghanistan,Myanmar,Somalia,Benin,Brazil,Burkina Faso,Burundi,Cambodia,Côte D’Ivoire,Indonesia,Lao Peoples Democratic Republic (The),Madagascar,Mauritius,Nicaragua,Sri Lanka,Tajikistan,Thailand,Viet Nam</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>Kenya,Uganda,Ethiopia,Nigeria,South Sudan,Somalia,Sudan (The),Mali,Niger (The),Burkina Faso,Chad,Eritrea,Mauritania,Syrian Arab Republic,Yemen</t>
+  </si>
+  <si>
+    <t>Kenya,Ethiopia,Ghana,Nigeria,Mozambique,Malawi,Rwanda,Sierra Leone,Drc,Benin,Burkina Faso,Cameroon,Côte D’Ivoire,Gabon,Togo</t>
+  </si>
+  <si>
+    <t>Kenya,Ethiopia,Bangladesh,Pakistan,Nepal,India</t>
+  </si>
+  <si>
+    <t>Tanzania,Ethiopia,Ghana,Rwanda,Pakistan,Sierra Leone,South Sudan,Lebanon,Kiribati</t>
+  </si>
+  <si>
+    <t>Kenya,Uganda,Bangladesh,Nigeria,Zambia,Rwanda,Pakistan</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>Ethiopia,India,Viet Nam,Peru</t>
+  </si>
+  <si>
+    <t>Kenya,Uganda,Tanzania,Ethiopia,Bangladesh,Ghana,Nigeria,Malawi,Pakistan,Sierra Leone,India,Zimbabwe,South Africa,South Sudan,Somalia,Sudan (The),Philippines (The),Lebanon,Morocco,Mongolia,Indonesia,Cambodia,Liberia,Thailand</t>
+  </si>
+  <si>
+    <t>Sierra Leone,Nepal,Myanmar,United Kingdom Of Great Britain And Northern Ireland (The),Lebanon</t>
+  </si>
+  <si>
+    <t>Uganda,Tanzania,Bangladesh,Nigeria,Malawi,Tajikistan,Mongolia,Uzbekistan,Papua New Guinea</t>
+  </si>
+  <si>
+    <t>Kenya,Uganda,Bangladesh,Nigeria,Zambia,Rwanda,Pakistan,Côte D’Ivoire</t>
+  </si>
+  <si>
+    <t>Uganda,Ethiopia</t>
+  </si>
+  <si>
+    <t>Bangladesh,Ghana,Nigeria,Nepal</t>
+  </si>
+  <si>
+    <t>Tanzania,Benin,Côte D’Ivoire,Cameroon</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Lead</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300552</t>
+  </si>
+  <si>
+    <t>Asia Regional Child Labour Programme</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300343</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1271,7 @@
     <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1206,6 +1391,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1391,7 +1583,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1506,8 +1698,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1550,8 +1757,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1564,8 +1772,11 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1599,6 +1810,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1609,7 +1821,17 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1634,6 +1856,21 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4B084"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1947,20 +2184,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{173F4EA4-DC3A-4C1B-81EE-634021F720DA}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.59765625" customWidth="1"/>
-    <col min="2" max="2" width="87.8984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="74.19921875" customWidth="1"/>
+    <col min="1" max="1" width="29.58203125" customWidth="1"/>
+    <col min="2" max="2" width="87.9140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="74.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -1971,7 +2208,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1979,7 +2216,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>319</v>
       </c>
@@ -1990,7 +2227,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1998,7 +2235,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>316</v>
       </c>
@@ -2006,7 +2243,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>320</v>
       </c>
@@ -2017,7 +2254,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2028,7 +2265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>346</v>
       </c>
@@ -2039,7 +2276,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>321</v>
       </c>
@@ -2050,7 +2287,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2058,7 +2295,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>328</v>
       </c>
@@ -2069,7 +2306,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>339</v>
       </c>
@@ -2077,7 +2314,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2088,7 +2325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>322</v>
       </c>
@@ -2099,7 +2336,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>329</v>
       </c>
@@ -2110,7 +2347,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>323</v>
       </c>
@@ -2121,7 +2358,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -2129,7 +2366,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>330</v>
       </c>
@@ -2140,7 +2377,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -2151,7 +2388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2159,7 +2396,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -2167,7 +2404,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>314</v>
       </c>
@@ -2178,7 +2415,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>327</v>
       </c>
@@ -2189,7 +2426,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -2200,7 +2437,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -2211,7 +2448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>331</v>
       </c>
@@ -2222,7 +2459,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>332</v>
       </c>
@@ -2230,7 +2467,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>342</v>
       </c>
@@ -2238,7 +2475,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -2246,7 +2483,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -2254,7 +2491,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>344</v>
       </c>
@@ -2262,7 +2499,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>309</v>
       </c>
@@ -2270,163 +2507,182 @@
         <v>310</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>317</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>333</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>405</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>335</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C37" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>313</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B38" t="s">
         <v>239</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C38" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="40" spans="1:3" ht="28" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>326</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C40" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="41" spans="1:3" ht="28" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>336</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C41" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="42" spans="1:3" ht="28" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>337</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C42" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>324</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C43" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="44" spans="1:3" ht="28" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>338</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C44" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="45" spans="1:3" ht="28" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>325</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C45" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>318</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C46" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>311</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>312</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C44" xr:uid="{97E336E5-A533-4260-8E56-96E4AAD413F4}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C44">
-      <sortCondition ref="A1:A44"/>
+  <autoFilter ref="A1:C46" xr:uid="{97E336E5-A533-4260-8E56-96E4AAD413F4}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C46">
+      <sortCondition ref="A1:A46"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"Columbia"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Columbia">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Columbia">
       <formula>NOT(ISERROR(SEARCH("Columbia",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="A1:A32 A34:A1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Calibri"&amp;10&amp;K000000OFFICIAL&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2435,20 +2691,20 @@
   <dimension ref="A1:I99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="55.3984375" customWidth="1"/>
+    <col min="2" max="2" width="55.4140625" customWidth="1"/>
     <col min="3" max="3" width="50.5" customWidth="1"/>
-    <col min="4" max="4" width="40.09765625" customWidth="1"/>
-    <col min="5" max="6" width="18.59765625" customWidth="1"/>
-    <col min="7" max="7" width="37.19921875" customWidth="1"/>
+    <col min="4" max="4" width="40.08203125" customWidth="1"/>
+    <col min="5" max="6" width="18.58203125" customWidth="1"/>
+    <col min="7" max="7" width="37.1640625" customWidth="1"/>
     <col min="8" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -2477,7 +2733,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>200574</v>
       </c>
@@ -2503,7 +2759,7 @@
         <v>15678567</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>201267</v>
       </c>
@@ -2532,7 +2788,7 @@
         <v>60200023.200000003</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>201879</v>
       </c>
@@ -2558,7 +2814,7 @@
         <v>24108119.600000001</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>201880</v>
       </c>
@@ -2587,7 +2843,7 @@
         <v>15484470</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>300704</v>
       </c>
@@ -2616,7 +2872,7 @@
         <v>1729643.3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>202749</v>
       </c>
@@ -2645,7 +2901,7 @@
         <v>11736364.4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>202766</v>
       </c>
@@ -2674,7 +2930,7 @@
         <v>5506031.7999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>202835</v>
       </c>
@@ -2703,7 +2959,7 @@
         <v>22713800.899999999</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>202960</v>
       </c>
@@ -2732,7 +2988,7 @@
         <v>17210000</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>203052</v>
       </c>
@@ -2761,7 +3017,7 @@
         <v>24057052.800000001</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>204773</v>
       </c>
@@ -2790,7 +3046,7 @@
         <v>11146113.300000001</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>203051</v>
       </c>
@@ -2819,7 +3075,7 @@
         <v>14274938.800000001</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>204153</v>
       </c>
@@ -2848,7 +3104,7 @@
         <v>15686534</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>203067</v>
       </c>
@@ -2877,7 +3133,7 @@
         <v>12287517.9</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>204764</v>
       </c>
@@ -2906,7 +3162,7 @@
         <v>139114489</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>300100</v>
       </c>
@@ -2935,7 +3191,7 @@
         <v>7502239.7000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>203529</v>
       </c>
@@ -2964,7 +3220,7 @@
         <v>19957172.100000001</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>203569</v>
       </c>
@@ -2993,7 +3249,7 @@
         <v>5748956.4000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>203752</v>
       </c>
@@ -3022,7 +3278,7 @@
         <v>13199472.699999999</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>203804</v>
       </c>
@@ -3051,7 +3307,7 @@
         <v>50566292.700000003</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>203835</v>
       </c>
@@ -3080,7 +3336,7 @@
         <v>19118231.600000001</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>203844</v>
       </c>
@@ -3109,7 +3365,7 @@
         <v>7779152.4000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>204836</v>
       </c>
@@ -3138,7 +3394,7 @@
         <v>1574613.4</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>203933</v>
       </c>
@@ -3167,7 +3423,7 @@
         <v>27196950</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>204133</v>
       </c>
@@ -3196,7 +3452,7 @@
         <v>1915865</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>300649</v>
       </c>
@@ -3225,7 +3481,7 @@
         <v>25678000</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>204291</v>
       </c>
@@ -3254,7 +3510,7 @@
         <v>4278920.5</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>203041</v>
       </c>
@@ -3283,7 +3539,7 @@
         <v>14783100</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>204324</v>
       </c>
@@ -3312,7 +3568,7 @@
         <v>12858249.5</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>300405</v>
       </c>
@@ -3341,7 +3597,7 @@
         <v>619341.4</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>204427</v>
       </c>
@@ -3370,7 +3626,7 @@
         <v>6232123.0999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>301135</v>
       </c>
@@ -3399,7 +3655,7 @@
         <v>111034.1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <v>204653</v>
       </c>
@@ -3428,7 +3684,7 @@
         <v>1959860.9</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>204725</v>
       </c>
@@ -3457,7 +3713,7 @@
         <v>6211834.2000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>204765</v>
       </c>
@@ -3486,7 +3742,7 @@
         <v>281590118.60000002</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>202568</v>
       </c>
@@ -3515,7 +3771,7 @@
         <v>12461864.199999999</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>204931</v>
       </c>
@@ -3544,7 +3800,7 @@
         <v>11099855</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>203050</v>
       </c>
@@ -3573,7 +3829,7 @@
         <v>19701355</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>301138</v>
       </c>
@@ -3602,7 +3858,7 @@
         <v>956166.6</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>205053</v>
       </c>
@@ -3631,7 +3887,7 @@
         <v>4544146</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>205103</v>
       </c>
@@ -3660,7 +3916,7 @@
         <v>4961891.2</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>205109</v>
       </c>
@@ -3689,7 +3945,7 @@
         <v>3759425.3</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>205121</v>
       </c>
@@ -3715,7 +3971,7 @@
         <v>8293978.7000000002</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>203089</v>
       </c>
@@ -3744,7 +4000,7 @@
         <v>9904337.3000000007</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>300049</v>
       </c>
@@ -3773,7 +4029,7 @@
         <v>9887920.5999999996</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>204322</v>
       </c>
@@ -3802,7 +4058,7 @@
         <v>28199097.699999999</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>300111</v>
       </c>
@@ -3831,7 +4087,7 @@
         <v>15624119</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>300123</v>
       </c>
@@ -3860,7 +4116,7 @@
         <v>15828676.300000001</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>300124</v>
       </c>
@@ -3889,7 +4145,7 @@
         <v>1758681.7</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>300125</v>
       </c>
@@ -3912,7 +4168,7 @@
         <v>4113266.7</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>300126</v>
       </c>
@@ -3941,7 +4197,7 @@
         <v>9916381.6999999993</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>300180</v>
       </c>
@@ -3967,7 +4223,7 @@
         <v>809778.6</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>204420</v>
       </c>
@@ -3996,7 +4252,7 @@
         <v>18916870.100000001</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>300632</v>
       </c>
@@ -4025,7 +4281,7 @@
         <v>6940534</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>300294</v>
       </c>
@@ -4054,7 +4310,7 @@
         <v>11948500</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>300341</v>
       </c>
@@ -4083,7 +4339,7 @@
         <v>377489579.80000001</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>300342</v>
       </c>
@@ -4109,7 +4365,7 @@
         <v>21448728.199999999</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>300343</v>
       </c>
@@ -4135,7 +4391,7 @@
         <v>22214869</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>300346</v>
       </c>
@@ -4164,7 +4420,7 @@
         <v>5197310.4000000004</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>300347</v>
       </c>
@@ -4193,7 +4449,7 @@
         <v>15800000</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>300384</v>
       </c>
@@ -4222,7 +4478,7 @@
         <v>11250000</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>300781</v>
       </c>
@@ -4251,7 +4507,7 @@
         <v>1397116</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>300446</v>
       </c>
@@ -4277,7 +4533,7 @@
         <v>11467782.699999999</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>300482</v>
       </c>
@@ -4306,7 +4562,7 @@
         <v>9015201.4000000004</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>300484</v>
       </c>
@@ -4332,7 +4588,7 @@
         <v>3740328</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>300504</v>
       </c>
@@ -4361,7 +4617,7 @@
         <v>7786167</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>300574</v>
       </c>
@@ -4390,7 +4646,7 @@
         <v>3906211</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>300615</v>
       </c>
@@ -4419,7 +4675,7 @@
         <v>393186.1</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>301134</v>
       </c>
@@ -4448,7 +4704,7 @@
         <v>957250.6</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>300644</v>
       </c>
@@ -4477,7 +4733,7 @@
         <v>7714532.0999999996</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>205271</v>
       </c>
@@ -4506,7 +4762,7 @@
         <v>41125249</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>300654</v>
       </c>
@@ -4535,7 +4791,7 @@
         <v>2103363.2999999998</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>300655</v>
       </c>
@@ -4564,7 +4820,7 @@
         <v>3056192.1</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>300656</v>
       </c>
@@ -4590,7 +4846,7 @@
         <v>1666092.8</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>300728</v>
       </c>
@@ -4619,7 +4875,7 @@
         <v>6357872.0999999996</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>300708</v>
       </c>
@@ -4645,7 +4901,7 @@
         <v>4691326.2</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>300211</v>
       </c>
@@ -4674,7 +4930,7 @@
         <v>4306194</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>300755</v>
       </c>
@@ -4703,7 +4959,7 @@
         <v>5603072.2999999998</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>300760</v>
       </c>
@@ -4726,7 +4982,7 @@
         <v>35050000</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>300769</v>
       </c>
@@ -4755,7 +5011,7 @@
         <v>547195</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>204867</v>
       </c>
@@ -4784,7 +5040,7 @@
         <v>76891056.900000006</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>300785</v>
       </c>
@@ -4813,7 +5069,7 @@
         <v>1631848.6</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>300815</v>
       </c>
@@ -4839,7 +5095,7 @@
         <v>12633595.9</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>300849</v>
       </c>
@@ -4868,7 +5124,7 @@
         <v>1079504.6000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>300966</v>
       </c>
@@ -4894,7 +5150,7 @@
         <v>6445497</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>301050</v>
       </c>
@@ -4917,7 +5173,7 @@
         <v>4700000</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>301067</v>
       </c>
@@ -4940,7 +5196,7 @@
         <v>32850000</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>301108</v>
       </c>
@@ -4969,7 +5225,7 @@
         <v>2833458.1</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>205288</v>
       </c>
@@ -4998,7 +5254,7 @@
         <v>10566684</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>301133</v>
       </c>
@@ -5027,7 +5283,7 @@
         <v>928203.3</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>203212</v>
       </c>
@@ -5056,7 +5312,7 @@
         <v>8900000</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>204415</v>
       </c>
@@ -5085,7 +5341,7 @@
         <v>20362597.199999999</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>301136</v>
       </c>
@@ -5114,7 +5370,7 @@
         <v>167296.29999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>301132</v>
       </c>
@@ -5143,7 +5399,7 @@
         <v>833464.7</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>301139</v>
       </c>
@@ -5172,7 +5428,7 @@
         <v>781523.6</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>301263</v>
       </c>
@@ -5198,7 +5454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>301290</v>
       </c>
@@ -5218,7 +5474,7 @@
         <v>4790000</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>301291</v>
       </c>
@@ -5242,10 +5498,2816 @@
       </c>
       <c r="I99" s="6">
         <v>8360472.9000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="SOUTH AFRICA">
+      <formula>NOT(ISERROR(SEARCH("SOUTH AFRICA",G1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Calibri"&amp;10&amp;K000000OFFICIAL&amp;1#</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83534B1A-76F9-4460-918B-21DF3189CA9D}">
+  <dimension ref="A1:L92"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="45.9140625" customWidth="1"/>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="4" max="5" width="18.58203125" customWidth="1"/>
+    <col min="6" max="6" width="50.5" customWidth="1"/>
+    <col min="7" max="7" width="15.75" customWidth="1"/>
+    <col min="8" max="8" width="12.9140625" customWidth="1"/>
+    <col min="9" max="9" width="12.4140625" customWidth="1"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>401</v>
+      </c>
+      <c r="H1" t="s">
+        <v>402</v>
+      </c>
+      <c r="I1" t="s">
+        <v>403</v>
+      </c>
+      <c r="J1" t="s">
+        <v>399</v>
+      </c>
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>203050</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="8">
+        <v>2013</v>
+      </c>
+      <c r="E2" s="8">
+        <v>2023</v>
+      </c>
+      <c r="F2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" t="s">
+        <v>369</v>
+      </c>
+      <c r="J2" t="s">
+        <v>400</v>
+      </c>
+      <c r="K2" s="5">
+        <v>19761356</v>
+      </c>
+      <c r="L2" s="9" t="str">
+        <f>HYPERLINK(CONCATENATE("https://devtracker.fcdo.gov.uk/projects/GB-1-",A2,"/summary"))</f>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-203050/summary</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>205288</v>
+      </c>
+      <c r="B3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="8">
+        <v>2016</v>
+      </c>
+      <c r="E3" s="8">
+        <v>2027</v>
+      </c>
+      <c r="F3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G3" t="s">
+        <v>392</v>
+      </c>
+      <c r="J3" t="s">
+        <v>400</v>
+      </c>
+      <c r="K3" s="5">
+        <v>36297928</v>
+      </c>
+      <c r="L3" s="9" t="str">
+        <f>HYPERLINK(CONCATENATE("https://devtracker.fcdo.gov.uk/projects/GB-1-",A3,"/summary"))</f>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-205288/summary</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>203051</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="8">
+        <v>2012</v>
+      </c>
+      <c r="E4" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" t="s">
+        <v>354</v>
+      </c>
+      <c r="J4" t="s">
+        <v>400</v>
+      </c>
+      <c r="K4" s="5">
+        <v>14994000</v>
+      </c>
+      <c r="L4" s="9" t="str">
+        <f>HYPERLINK(CONCATENATE("https://devtracker.fcdo.gov.uk/projects/GB-1-",A4,"/summary"))</f>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-203051/summary</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>204764</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="8">
+        <v>2017</v>
+      </c>
+      <c r="E5" s="8">
+        <v>2023</v>
+      </c>
+      <c r="F5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G5" t="s">
+        <v>356</v>
+      </c>
+      <c r="J5" t="s">
+        <v>400</v>
+      </c>
+      <c r="K5" s="5">
+        <v>139261429</v>
+      </c>
+      <c r="L5" s="9" t="str">
+        <f>HYPERLINK(CONCATENATE("https://devtracker.fcdo.gov.uk/projects/GB-1-",A5,"/summary"))</f>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-204764/summary</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>204773</v>
+      </c>
+      <c r="B6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="8">
+        <v>2016</v>
+      </c>
+      <c r="E6" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G6" t="s">
+        <v>353</v>
+      </c>
+      <c r="J6" t="s">
+        <v>400</v>
+      </c>
+      <c r="K6" s="5">
+        <v>15500000</v>
+      </c>
+      <c r="L6" s="9" t="str">
+        <f>HYPERLINK(CONCATENATE("https://devtracker.fcdo.gov.uk/projects/GB-1-",A6,"/summary"))</f>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-204773/summary</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>300728</v>
+      </c>
+      <c r="B7" t="s">
+        <v>246</v>
+      </c>
+      <c r="D7" s="8">
+        <v>2019</v>
+      </c>
+      <c r="E7" s="8">
+        <v>2024</v>
+      </c>
+      <c r="F7" t="s">
+        <v>247</v>
+      </c>
+      <c r="G7" t="s">
+        <v>386</v>
+      </c>
+      <c r="J7" t="s">
+        <v>400</v>
+      </c>
+      <c r="K7" s="5">
+        <v>38000000</v>
+      </c>
+      <c r="L7" s="9" t="str">
+        <f>HYPERLINK(CONCATENATE("https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-",A7,"/summary"))</f>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300728/summary</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>300769</v>
+      </c>
+      <c r="B8" t="s">
+        <v>254</v>
+      </c>
+      <c r="D8" s="8">
+        <v>2019</v>
+      </c>
+      <c r="E8" s="8">
+        <v>2026</v>
+      </c>
+      <c r="F8" t="s">
+        <v>255</v>
+      </c>
+      <c r="G8" t="s">
+        <v>388</v>
+      </c>
+      <c r="J8" t="s">
+        <v>400</v>
+      </c>
+      <c r="K8" s="5">
+        <v>20500000</v>
+      </c>
+      <c r="L8" s="9" t="str">
+        <f>HYPERLINK(CONCATENATE("https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-",A8,"/summary"))</f>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300769/summary</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>301133</v>
+      </c>
+      <c r="B9" t="s">
+        <v>283</v>
+      </c>
+      <c r="D9" s="8">
+        <v>2020</v>
+      </c>
+      <c r="E9" s="8">
+        <v>2026</v>
+      </c>
+      <c r="F9" t="s">
+        <v>284</v>
+      </c>
+      <c r="G9" t="s">
+        <v>393</v>
+      </c>
+      <c r="J9" t="s">
+        <v>400</v>
+      </c>
+      <c r="K9" s="5">
+        <v>7682213</v>
+      </c>
+      <c r="L9" s="9" t="str">
+        <f>HYPERLINK(CONCATENATE("https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-",A9,"/summary"))</f>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-301133/summary</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>301134</v>
+      </c>
+      <c r="B10" t="s">
+        <v>286</v>
+      </c>
+      <c r="D10" s="8">
+        <v>2020</v>
+      </c>
+      <c r="E10" s="8">
+        <v>2026</v>
+      </c>
+      <c r="F10" t="s">
+        <v>287</v>
+      </c>
+      <c r="G10" t="s">
+        <v>381</v>
+      </c>
+      <c r="J10" t="s">
+        <v>400</v>
+      </c>
+      <c r="K10" s="5">
+        <v>6941624</v>
+      </c>
+      <c r="L10" s="9" t="str">
+        <f>HYPERLINK(CONCATENATE("https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-",A10,"/summary"))</f>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-301134/summary</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>300704</v>
+      </c>
+      <c r="B11" t="s">
+        <v>239</v>
+      </c>
+      <c r="D11" s="8">
+        <v>2019</v>
+      </c>
+      <c r="E11" s="8">
+        <v>2025</v>
+      </c>
+      <c r="F11" t="s">
+        <v>240</v>
+      </c>
+      <c r="G11" t="s">
+        <v>350</v>
+      </c>
+      <c r="J11" t="s">
+        <v>400</v>
+      </c>
+      <c r="K11" s="5">
+        <v>32207530</v>
+      </c>
+      <c r="L11" s="9" t="str">
+        <f>HYPERLINK(CONCATENATE("https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-",A11,"/summary"))</f>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300704/summary</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>204153</v>
+      </c>
+      <c r="B12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="8">
+        <v>2015</v>
+      </c>
+      <c r="E12" s="8">
+        <v>2025</v>
+      </c>
+      <c r="F12" t="s">
+        <v>115</v>
+      </c>
+      <c r="G12" t="s">
+        <v>355</v>
+      </c>
+      <c r="J12" t="s">
+        <v>400</v>
+      </c>
+      <c r="K12" s="5">
+        <v>22300000</v>
+      </c>
+      <c r="L12" s="9" t="str">
+        <f t="shared" ref="L12:L45" si="0">HYPERLINK(CONCATENATE("https://devtracker.fcdo.gov.uk/projects/GB-1-",A12,"/summary"))</f>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-204153/summary</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>203041</v>
+      </c>
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="8">
+        <v>2012</v>
+      </c>
+      <c r="E13" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" t="s">
+        <v>362</v>
+      </c>
+      <c r="J13" t="s">
+        <v>400</v>
+      </c>
+      <c r="K13" s="5">
+        <v>15376244</v>
+      </c>
+      <c r="L13" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-203041/summary</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>204931</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="8">
+        <v>2016</v>
+      </c>
+      <c r="E14" s="8">
+        <v>2023</v>
+      </c>
+      <c r="F14" t="s">
+        <v>152</v>
+      </c>
+      <c r="G14" t="s">
+        <v>368</v>
+      </c>
+      <c r="J14" t="s">
+        <v>400</v>
+      </c>
+      <c r="K14" s="5">
+        <v>12250000</v>
+      </c>
+      <c r="L14" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-204931/summary</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>205271</v>
+      </c>
+      <c r="B15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D15" s="8">
+        <v>2016</v>
+      </c>
+      <c r="E15" s="8">
+        <v>2023</v>
+      </c>
+      <c r="F15" t="s">
+        <v>163</v>
+      </c>
+      <c r="G15" t="s">
+        <v>383</v>
+      </c>
+      <c r="J15" t="s">
+        <v>400</v>
+      </c>
+      <c r="K15" s="5">
+        <v>44925736</v>
+      </c>
+      <c r="L15" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-205271/summary</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>200574</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="8">
+        <v>2009</v>
+      </c>
+      <c r="E16" s="8">
+        <v>2023</v>
+      </c>
+      <c r="F16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" t="s">
+        <v>347</v>
+      </c>
+      <c r="J16" t="s">
+        <v>400</v>
+      </c>
+      <c r="K16" s="5">
+        <v>17162788</v>
+      </c>
+      <c r="L16" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-200574/summary</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>201267</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="8">
+        <v>2009</v>
+      </c>
+      <c r="E17" s="8">
+        <v>2027</v>
+      </c>
+      <c r="F17" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" t="s">
+        <v>348</v>
+      </c>
+      <c r="J17" t="s">
+        <v>400</v>
+      </c>
+      <c r="K17" s="5">
+        <v>77000000</v>
+      </c>
+      <c r="L17" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-201267/summary</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>201879</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="8">
+        <v>2013</v>
+      </c>
+      <c r="E18" s="8">
+        <v>2023</v>
+      </c>
+      <c r="F18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" t="s">
+        <v>347</v>
+      </c>
+      <c r="J18" t="s">
+        <v>400</v>
+      </c>
+      <c r="K18" s="5">
+        <v>40501000</v>
+      </c>
+      <c r="L18" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-201879/summary</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>201880</v>
+      </c>
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="8">
+        <v>2013</v>
+      </c>
+      <c r="E19" s="8">
+        <v>2024</v>
+      </c>
+      <c r="F19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" t="s">
+        <v>349</v>
+      </c>
+      <c r="J19" t="s">
+        <v>400</v>
+      </c>
+      <c r="K19" s="5">
+        <v>22500000</v>
+      </c>
+      <c r="L19" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-201880/summary</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>202568</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="8">
+        <v>2011</v>
+      </c>
+      <c r="E20" s="8">
+        <v>2025</v>
+      </c>
+      <c r="F20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" t="s">
+        <v>367</v>
+      </c>
+      <c r="J20" t="s">
+        <v>400</v>
+      </c>
+      <c r="K20" s="5">
+        <v>24600000</v>
+      </c>
+      <c r="L20" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-202568/summary</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>202766</v>
+      </c>
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="8">
+        <v>2012</v>
+      </c>
+      <c r="E21" s="8">
+        <v>2024</v>
+      </c>
+      <c r="F21" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" t="s">
+        <v>348</v>
+      </c>
+      <c r="J21" t="s">
+        <v>400</v>
+      </c>
+      <c r="K21" s="5">
+        <v>6128571</v>
+      </c>
+      <c r="L21" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-202766/summary</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>202835</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="8">
+        <v>2011</v>
+      </c>
+      <c r="E22" s="8">
+        <v>2025</v>
+      </c>
+      <c r="F22" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" t="s">
+        <v>351</v>
+      </c>
+      <c r="J22" t="s">
+        <v>400</v>
+      </c>
+      <c r="K22" s="5">
+        <v>36640000</v>
+      </c>
+      <c r="L22" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-202835/summary</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>202960</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="8">
+        <v>2011</v>
+      </c>
+      <c r="E23" s="8">
+        <v>2025</v>
+      </c>
+      <c r="F23" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" t="s">
+        <v>348</v>
+      </c>
+      <c r="J23" t="s">
+        <v>400</v>
+      </c>
+      <c r="K23" s="5">
+        <v>19835986</v>
+      </c>
+      <c r="L23" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-202960/summary</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>203052</v>
+      </c>
+      <c r="B24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="8">
+        <v>2011</v>
+      </c>
+      <c r="E24" s="8">
+        <v>2029</v>
+      </c>
+      <c r="F24" t="s">
+        <v>81</v>
+      </c>
+      <c r="G24" t="s">
+        <v>352</v>
+      </c>
+      <c r="J24" t="s">
+        <v>400</v>
+      </c>
+      <c r="K24" s="5">
+        <v>31131042</v>
+      </c>
+      <c r="L24" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-203052/summary</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>203212</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="8">
+        <v>2012</v>
+      </c>
+      <c r="E25" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F25" t="s">
+        <v>90</v>
+      </c>
+      <c r="G25" t="s">
+        <v>394</v>
+      </c>
+      <c r="J25" t="s">
+        <v>400</v>
+      </c>
+      <c r="K25" s="5">
+        <v>9800000</v>
+      </c>
+      <c r="L25" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-203212/summary</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>203529</v>
+      </c>
+      <c r="B26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="8">
+        <v>2013</v>
+      </c>
+      <c r="E26" s="8">
+        <v>2024</v>
+      </c>
+      <c r="F26" t="s">
+        <v>93</v>
+      </c>
+      <c r="G26" t="s">
+        <v>358</v>
+      </c>
+      <c r="J26" t="s">
+        <v>400</v>
+      </c>
+      <c r="K26" s="5">
+        <v>30896804</v>
+      </c>
+      <c r="L26" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-203529/summary</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>203569</v>
+      </c>
+      <c r="B27" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" s="8">
+        <v>2013</v>
+      </c>
+      <c r="E27" s="8">
+        <v>2023</v>
+      </c>
+      <c r="F27" t="s">
+        <v>97</v>
+      </c>
+      <c r="G27" t="s">
+        <v>348</v>
+      </c>
+      <c r="J27" t="s">
+        <v>400</v>
+      </c>
+      <c r="K27" s="5">
+        <v>20000000</v>
+      </c>
+      <c r="L27" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-203569/summary</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>203752</v>
+      </c>
+      <c r="B28" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" s="8">
+        <v>2015</v>
+      </c>
+      <c r="E28" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F28" t="s">
+        <v>100</v>
+      </c>
+      <c r="G28" t="s">
+        <v>348</v>
+      </c>
+      <c r="J28" t="s">
+        <v>400</v>
+      </c>
+      <c r="K28" s="5">
+        <v>16248812</v>
+      </c>
+      <c r="L28" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-203752/summary</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>203844</v>
+      </c>
+      <c r="B29" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" s="8">
+        <v>2014</v>
+      </c>
+      <c r="E29" s="8">
+        <v>2023</v>
+      </c>
+      <c r="F29" t="s">
+        <v>108</v>
+      </c>
+      <c r="G29" t="s">
+        <v>359</v>
+      </c>
+      <c r="J29" t="s">
+        <v>400</v>
+      </c>
+      <c r="K29" s="5">
+        <v>18000000</v>
+      </c>
+      <c r="L29" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-203844/summary</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>203933</v>
+      </c>
+      <c r="B30" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" s="8">
+        <v>2012</v>
+      </c>
+      <c r="E30" s="8">
+        <v>2024</v>
+      </c>
+      <c r="F30" t="s">
+        <v>111</v>
+      </c>
+      <c r="G30" t="s">
+        <v>348</v>
+      </c>
+      <c r="J30" t="s">
+        <v>400</v>
+      </c>
+      <c r="K30" s="5">
+        <v>29904657</v>
+      </c>
+      <c r="L30" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-203933/summary</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>204133</v>
+      </c>
+      <c r="B31" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" s="8">
+        <v>2013</v>
+      </c>
+      <c r="E31" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F31" t="s">
+        <v>113</v>
+      </c>
+      <c r="G31" t="s">
+        <v>348</v>
+      </c>
+      <c r="J31" t="s">
+        <v>400</v>
+      </c>
+      <c r="K31" s="5">
+        <v>3103308</v>
+      </c>
+      <c r="L31" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-204133/summary</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>204291</v>
+      </c>
+      <c r="B32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" s="8">
+        <v>2014</v>
+      </c>
+      <c r="E32" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F32" t="s">
+        <v>117</v>
+      </c>
+      <c r="G32" t="s">
+        <v>348</v>
+      </c>
+      <c r="J32" t="s">
+        <v>400</v>
+      </c>
+      <c r="K32" s="5">
+        <v>4914002</v>
+      </c>
+      <c r="L32" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-204291/summary</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>204322</v>
+      </c>
+      <c r="B33" t="s">
+        <v>119</v>
+      </c>
+      <c r="D33" s="8">
+        <v>2014</v>
+      </c>
+      <c r="E33" s="8">
+        <v>2025</v>
+      </c>
+      <c r="F33" t="s">
+        <v>120</v>
+      </c>
+      <c r="G33" t="s">
+        <v>374</v>
+      </c>
+      <c r="J33" t="s">
+        <v>400</v>
+      </c>
+      <c r="K33" s="5">
+        <v>37660852</v>
+      </c>
+      <c r="L33" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-204322/summary</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>204324</v>
+      </c>
+      <c r="B34" t="s">
+        <v>122</v>
+      </c>
+      <c r="D34" s="8">
+        <v>2014</v>
+      </c>
+      <c r="E34" s="8">
+        <v>2025</v>
+      </c>
+      <c r="F34" t="s">
+        <v>123</v>
+      </c>
+      <c r="G34" t="s">
+        <v>348</v>
+      </c>
+      <c r="J34" t="s">
+        <v>400</v>
+      </c>
+      <c r="K34" s="5">
+        <v>15000000</v>
+      </c>
+      <c r="L34" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-204324/summary</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>204415</v>
+      </c>
+      <c r="B35" t="s">
+        <v>124</v>
+      </c>
+      <c r="D35" s="8">
+        <v>2014</v>
+      </c>
+      <c r="E35" s="8">
+        <v>2025</v>
+      </c>
+      <c r="F35" t="s">
+        <v>125</v>
+      </c>
+      <c r="G35" t="s">
+        <v>395</v>
+      </c>
+      <c r="J35" t="s">
+        <v>400</v>
+      </c>
+      <c r="K35" s="5">
+        <v>40150002</v>
+      </c>
+      <c r="L35" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-204415/summary</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>204420</v>
+      </c>
+      <c r="B36" t="s">
+        <v>128</v>
+      </c>
+      <c r="D36" s="8">
+        <v>2014</v>
+      </c>
+      <c r="E36" s="8">
+        <v>2025</v>
+      </c>
+      <c r="F36" t="s">
+        <v>129</v>
+      </c>
+      <c r="G36" t="s">
+        <v>375</v>
+      </c>
+      <c r="J36" t="s">
+        <v>400</v>
+      </c>
+      <c r="K36" s="5">
+        <v>35000000</v>
+      </c>
+      <c r="L36" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-204420/summary</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>204427</v>
+      </c>
+      <c r="B37" t="s">
+        <v>131</v>
+      </c>
+      <c r="D37" s="8">
+        <v>2015</v>
+      </c>
+      <c r="E37" s="8">
+        <v>2021</v>
+      </c>
+      <c r="F37" t="s">
+        <v>132</v>
+      </c>
+      <c r="G37" t="s">
+        <v>364</v>
+      </c>
+      <c r="J37" t="s">
+        <v>400</v>
+      </c>
+      <c r="K37" s="5">
+        <v>6500000</v>
+      </c>
+      <c r="L37" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-204427/summary</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>204725</v>
+      </c>
+      <c r="B38" t="s">
+        <v>137</v>
+      </c>
+      <c r="D38" s="8">
+        <v>2014</v>
+      </c>
+      <c r="E38" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F38" t="s">
+        <v>138</v>
+      </c>
+      <c r="G38" t="s">
+        <v>366</v>
+      </c>
+      <c r="J38" t="s">
+        <v>400</v>
+      </c>
+      <c r="K38" s="5">
+        <v>6782899</v>
+      </c>
+      <c r="L38" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-204725/summary</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>204765</v>
+      </c>
+      <c r="B39" t="s">
+        <v>141</v>
+      </c>
+      <c r="D39" s="8">
+        <v>2014</v>
+      </c>
+      <c r="E39" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F39" t="s">
+        <v>142</v>
+      </c>
+      <c r="G39" t="s">
+        <v>348</v>
+      </c>
+      <c r="J39" t="s">
+        <v>400</v>
+      </c>
+      <c r="K39" s="5">
+        <v>317065080</v>
+      </c>
+      <c r="L39" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-204765/summary</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>204836</v>
+      </c>
+      <c r="B40" t="s">
+        <v>146</v>
+      </c>
+      <c r="D40" s="8">
+        <v>2017</v>
+      </c>
+      <c r="E40" s="8">
+        <v>2027</v>
+      </c>
+      <c r="F40" t="s">
+        <v>147</v>
+      </c>
+      <c r="G40" t="s">
+        <v>360</v>
+      </c>
+      <c r="J40" t="s">
+        <v>400</v>
+      </c>
+      <c r="K40" s="5">
+        <v>12000000</v>
+      </c>
+      <c r="L40" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-204836/summary</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>204867</v>
+      </c>
+      <c r="B41" t="s">
+        <v>149</v>
+      </c>
+      <c r="D41" s="8">
+        <v>2015</v>
+      </c>
+      <c r="E41" s="8">
+        <v>2024</v>
+      </c>
+      <c r="F41" t="s">
+        <v>150</v>
+      </c>
+      <c r="G41" t="s">
+        <v>389</v>
+      </c>
+      <c r="J41" t="s">
+        <v>400</v>
+      </c>
+      <c r="K41" s="5">
+        <v>99193930</v>
+      </c>
+      <c r="L41" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-204867/summary</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>205053</v>
+      </c>
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="8">
+        <v>2015</v>
+      </c>
+      <c r="E42" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F42" t="s">
+        <v>153</v>
+      </c>
+      <c r="G42" t="s">
+        <v>371</v>
+      </c>
+      <c r="J42" t="s">
+        <v>400</v>
+      </c>
+      <c r="K42" s="5">
+        <v>4900000</v>
+      </c>
+      <c r="L42" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-205053/summary</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>205103</v>
+      </c>
+      <c r="B43" t="s">
+        <v>154</v>
+      </c>
+      <c r="D43" s="8">
+        <v>2015</v>
+      </c>
+      <c r="E43" s="8">
+        <v>2021</v>
+      </c>
+      <c r="F43" t="s">
+        <v>155</v>
+      </c>
+      <c r="G43" t="s">
+        <v>372</v>
+      </c>
+      <c r="J43" t="s">
+        <v>400</v>
+      </c>
+      <c r="K43" s="5">
+        <v>5000000</v>
+      </c>
+      <c r="L43" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-205103/summary</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>205109</v>
+      </c>
+      <c r="B44" t="s">
+        <v>157</v>
+      </c>
+      <c r="D44" s="8">
+        <v>2016</v>
+      </c>
+      <c r="E44" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F44" t="s">
+        <v>158</v>
+      </c>
+      <c r="G44" t="s">
+        <v>348</v>
+      </c>
+      <c r="J44" t="s">
+        <v>400</v>
+      </c>
+      <c r="K44" s="5">
+        <v>4500000</v>
+      </c>
+      <c r="L44" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-205109/summary</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>205121</v>
+      </c>
+      <c r="B45" t="s">
+        <v>159</v>
+      </c>
+      <c r="D45" s="8">
+        <v>2016</v>
+      </c>
+      <c r="E45" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F45" t="s">
+        <v>160</v>
+      </c>
+      <c r="G45" t="s">
+        <v>373</v>
+      </c>
+      <c r="J45" t="s">
+        <v>400</v>
+      </c>
+      <c r="K45" s="5">
+        <v>9646279</v>
+      </c>
+      <c r="L45" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-1-205121/summary</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>300049</v>
+      </c>
+      <c r="B46" t="s">
+        <v>167</v>
+      </c>
+      <c r="D46" s="8">
+        <v>2016</v>
+      </c>
+      <c r="E46" s="8">
+        <v>2024</v>
+      </c>
+      <c r="F46" t="s">
+        <v>168</v>
+      </c>
+      <c r="G46" t="s">
+        <v>348</v>
+      </c>
+      <c r="J46" t="s">
+        <v>400</v>
+      </c>
+      <c r="K46" s="5">
+        <v>15300000</v>
+      </c>
+      <c r="L46" s="9" t="str">
+        <f t="shared" ref="L46:L92" si="1">HYPERLINK(CONCATENATE("https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-",A46,"/summary"))</f>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300049/summary</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>300100</v>
+      </c>
+      <c r="B47" t="s">
+        <v>169</v>
+      </c>
+      <c r="D47" s="8">
+        <v>2017</v>
+      </c>
+      <c r="E47" s="8">
+        <v>2025</v>
+      </c>
+      <c r="F47" t="s">
+        <v>170</v>
+      </c>
+      <c r="G47" t="s">
+        <v>357</v>
+      </c>
+      <c r="J47" t="s">
+        <v>400</v>
+      </c>
+      <c r="K47" s="5">
+        <v>29000000</v>
+      </c>
+      <c r="L47" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300100/summary</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>300111</v>
+      </c>
+      <c r="B48" t="s">
+        <v>173</v>
+      </c>
+      <c r="D48" s="8">
+        <v>2016</v>
+      </c>
+      <c r="E48" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F48" t="s">
+        <v>174</v>
+      </c>
+      <c r="G48" t="s">
+        <v>348</v>
+      </c>
+      <c r="J48" t="s">
+        <v>400</v>
+      </c>
+      <c r="K48" s="5">
+        <v>18199769</v>
+      </c>
+      <c r="L48" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300111/summary</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>300123</v>
+      </c>
+      <c r="B49" t="s">
+        <v>175</v>
+      </c>
+      <c r="D49" s="8">
+        <v>2016</v>
+      </c>
+      <c r="E49" s="8">
+        <v>2023</v>
+      </c>
+      <c r="F49" t="s">
+        <v>176</v>
+      </c>
+      <c r="G49" t="s">
+        <v>348</v>
+      </c>
+      <c r="J49" t="s">
+        <v>400</v>
+      </c>
+      <c r="K49" s="5">
+        <v>40150001</v>
+      </c>
+      <c r="L49" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300123/summary</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>300124</v>
+      </c>
+      <c r="B50" t="s">
+        <v>177</v>
+      </c>
+      <c r="D50" s="8">
+        <v>2017</v>
+      </c>
+      <c r="E50" s="8">
+        <v>2024</v>
+      </c>
+      <c r="F50" t="s">
+        <v>178</v>
+      </c>
+      <c r="G50" t="s">
+        <v>348</v>
+      </c>
+      <c r="J50" t="s">
+        <v>400</v>
+      </c>
+      <c r="K50" s="5">
+        <v>24650000</v>
+      </c>
+      <c r="L50" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300124/summary</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>300125</v>
+      </c>
+      <c r="B51" t="s">
+        <v>179</v>
+      </c>
+      <c r="D51" s="8">
+        <v>2019</v>
+      </c>
+      <c r="E51" s="8">
+        <v>2025</v>
+      </c>
+      <c r="F51" t="s">
+        <v>180</v>
+      </c>
+      <c r="G51" t="s">
+        <v>347</v>
+      </c>
+      <c r="J51" t="s">
+        <v>400</v>
+      </c>
+      <c r="K51" s="5">
+        <v>38000000</v>
+      </c>
+      <c r="L51" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300125/summary</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>300126</v>
+      </c>
+      <c r="B52" t="s">
+        <v>181</v>
+      </c>
+      <c r="D52" s="8">
+        <v>2018</v>
+      </c>
+      <c r="E52" s="8">
+        <v>2027</v>
+      </c>
+      <c r="F52" t="s">
+        <v>182</v>
+      </c>
+      <c r="G52" t="s">
+        <v>348</v>
+      </c>
+      <c r="J52" t="s">
+        <v>400</v>
+      </c>
+      <c r="K52" s="5">
+        <v>102500000</v>
+      </c>
+      <c r="L52" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300126/summary</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>300180</v>
+      </c>
+      <c r="B53" t="s">
+        <v>184</v>
+      </c>
+      <c r="D53" s="8">
+        <v>2018</v>
+      </c>
+      <c r="E53" s="8">
+        <v>2026</v>
+      </c>
+      <c r="F53" t="s">
+        <v>185</v>
+      </c>
+      <c r="G53" t="s">
+        <v>347</v>
+      </c>
+      <c r="J53" t="s">
+        <v>400</v>
+      </c>
+      <c r="K53" s="5">
+        <v>32750000</v>
+      </c>
+      <c r="L53" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300180/summary</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>300294</v>
+      </c>
+      <c r="B54" t="s">
+        <v>189</v>
+      </c>
+      <c r="D54" s="8">
+        <v>2016</v>
+      </c>
+      <c r="E54" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F54" t="s">
+        <v>190</v>
+      </c>
+      <c r="G54" t="s">
+        <v>348</v>
+      </c>
+      <c r="J54" t="s">
+        <v>400</v>
+      </c>
+      <c r="K54" s="5">
+        <v>12923500</v>
+      </c>
+      <c r="L54" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300294/summary</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>300341</v>
+      </c>
+      <c r="B55" t="s">
+        <v>191</v>
+      </c>
+      <c r="D55" s="8">
+        <v>2017</v>
+      </c>
+      <c r="E55" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F55" t="s">
+        <v>192</v>
+      </c>
+      <c r="G55" t="s">
+        <v>348</v>
+      </c>
+      <c r="J55" t="s">
+        <v>400</v>
+      </c>
+      <c r="K55" s="5">
+        <v>391033790</v>
+      </c>
+      <c r="L55" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300341/summary</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>300342</v>
+      </c>
+      <c r="B56" t="s">
+        <v>193</v>
+      </c>
+      <c r="D56" s="8">
+        <v>2017</v>
+      </c>
+      <c r="E56" s="8">
+        <v>2024</v>
+      </c>
+      <c r="F56" t="s">
+        <v>194</v>
+      </c>
+      <c r="G56" t="s">
+        <v>347</v>
+      </c>
+      <c r="J56" t="s">
+        <v>400</v>
+      </c>
+      <c r="K56" s="5">
+        <v>26805635</v>
+      </c>
+      <c r="L56" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300342/summary</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>300343</v>
+      </c>
+      <c r="B57" t="s">
+        <v>195</v>
+      </c>
+      <c r="D57" s="8">
+        <v>2018</v>
+      </c>
+      <c r="E57" s="8">
+        <v>2023</v>
+      </c>
+      <c r="F57" t="s">
+        <v>196</v>
+      </c>
+      <c r="G57" t="s">
+        <v>347</v>
+      </c>
+      <c r="J57" t="s">
+        <v>400</v>
+      </c>
+      <c r="K57" s="5">
+        <v>30214869</v>
+      </c>
+      <c r="L57" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300343/summary</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>300346</v>
+      </c>
+      <c r="B58" t="s">
+        <v>197</v>
+      </c>
+      <c r="D58" s="8">
+        <v>2018</v>
+      </c>
+      <c r="E58" s="8">
+        <v>2026</v>
+      </c>
+      <c r="F58" t="s">
+        <v>198</v>
+      </c>
+      <c r="G58" t="s">
+        <v>348</v>
+      </c>
+      <c r="J58" t="s">
+        <v>400</v>
+      </c>
+      <c r="K58" s="5">
+        <v>10687612</v>
+      </c>
+      <c r="L58" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300346/summary</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>300347</v>
+      </c>
+      <c r="B59" t="s">
+        <v>199</v>
+      </c>
+      <c r="D59" s="8">
+        <v>2018</v>
+      </c>
+      <c r="E59" s="8">
+        <v>2023</v>
+      </c>
+      <c r="F59" t="s">
+        <v>200</v>
+      </c>
+      <c r="G59" t="s">
+        <v>348</v>
+      </c>
+      <c r="J59" t="s">
+        <v>400</v>
+      </c>
+      <c r="K59" s="5">
+        <v>23500000</v>
+      </c>
+      <c r="L59" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300347/summary</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>300384</v>
+      </c>
+      <c r="B60" t="s">
+        <v>201</v>
+      </c>
+      <c r="D60" s="8">
+        <v>2017</v>
+      </c>
+      <c r="E60" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F60" t="s">
+        <v>202</v>
+      </c>
+      <c r="G60" t="s">
+        <v>348</v>
+      </c>
+      <c r="J60" t="s">
+        <v>400</v>
+      </c>
+      <c r="K60" s="5">
+        <v>11250000</v>
+      </c>
+      <c r="L60" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300384/summary</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>300405</v>
+      </c>
+      <c r="B61" t="s">
+        <v>203</v>
+      </c>
+      <c r="D61" s="8">
+        <v>2017</v>
+      </c>
+      <c r="E61" s="8">
+        <v>2026</v>
+      </c>
+      <c r="F61" t="s">
+        <v>204</v>
+      </c>
+      <c r="G61" t="s">
+        <v>363</v>
+      </c>
+      <c r="J61" t="s">
+        <v>400</v>
+      </c>
+      <c r="K61" s="5">
+        <v>26500000</v>
+      </c>
+      <c r="L61" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300405/summary</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>300446</v>
+      </c>
+      <c r="B62" t="s">
+        <v>206</v>
+      </c>
+      <c r="D62" s="8">
+        <v>2017</v>
+      </c>
+      <c r="E62" s="8">
+        <v>2026</v>
+      </c>
+      <c r="F62" t="s">
+        <v>207</v>
+      </c>
+      <c r="G62" t="s">
+        <v>347</v>
+      </c>
+      <c r="J62" t="s">
+        <v>400</v>
+      </c>
+      <c r="K62" s="5">
+        <v>15500000</v>
+      </c>
+      <c r="L62" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300446/summary</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>300482</v>
+      </c>
+      <c r="B63" t="s">
+        <v>208</v>
+      </c>
+      <c r="D63" s="8">
+        <v>2018</v>
+      </c>
+      <c r="E63" s="8">
+        <v>2023</v>
+      </c>
+      <c r="F63" t="s">
+        <v>209</v>
+      </c>
+      <c r="G63" t="s">
+        <v>378</v>
+      </c>
+      <c r="J63" t="s">
+        <v>400</v>
+      </c>
+      <c r="K63" s="5">
+        <v>38053854</v>
+      </c>
+      <c r="L63" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300482/summary</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>300484</v>
+      </c>
+      <c r="B64" t="s">
+        <v>211</v>
+      </c>
+      <c r="D64" s="8">
+        <v>2018</v>
+      </c>
+      <c r="E64" s="8">
+        <v>2024</v>
+      </c>
+      <c r="F64" t="s">
+        <v>212</v>
+      </c>
+      <c r="G64" t="s">
+        <v>347</v>
+      </c>
+      <c r="J64" t="s">
+        <v>400</v>
+      </c>
+      <c r="K64" s="5">
+        <v>18099997</v>
+      </c>
+      <c r="L64" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300484/summary</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>300504</v>
+      </c>
+      <c r="B65" t="s">
+        <v>213</v>
+      </c>
+      <c r="D65" s="8">
+        <v>2018</v>
+      </c>
+      <c r="E65" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F65" t="s">
+        <v>214</v>
+      </c>
+      <c r="G65" t="s">
+        <v>379</v>
+      </c>
+      <c r="J65" t="s">
+        <v>400</v>
+      </c>
+      <c r="K65" s="5">
+        <v>12600000</v>
+      </c>
+      <c r="L65" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300504/summary</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>300574</v>
+      </c>
+      <c r="B66" t="s">
+        <v>216</v>
+      </c>
+      <c r="D66" s="8">
+        <v>2018</v>
+      </c>
+      <c r="E66" s="8">
+        <v>2023</v>
+      </c>
+      <c r="F66" t="s">
+        <v>217</v>
+      </c>
+      <c r="G66" t="s">
+        <v>380</v>
+      </c>
+      <c r="J66" t="s">
+        <v>400</v>
+      </c>
+      <c r="K66" s="5">
+        <v>9224743</v>
+      </c>
+      <c r="L66" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300574/summary</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>300615</v>
+      </c>
+      <c r="B67" t="s">
+        <v>220</v>
+      </c>
+      <c r="D67" s="8">
+        <v>2018</v>
+      </c>
+      <c r="E67" s="8">
+        <v>2025</v>
+      </c>
+      <c r="F67" t="s">
+        <v>221</v>
+      </c>
+      <c r="G67" t="s">
+        <v>348</v>
+      </c>
+      <c r="J67" t="s">
+        <v>400</v>
+      </c>
+      <c r="K67" s="5">
+        <v>3505619</v>
+      </c>
+      <c r="L67" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300615/summary</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>300632</v>
+      </c>
+      <c r="B68" t="s">
+        <v>222</v>
+      </c>
+      <c r="D68" s="8">
+        <v>2019</v>
+      </c>
+      <c r="E68" s="8">
+        <v>2025</v>
+      </c>
+      <c r="F68" t="s">
+        <v>223</v>
+      </c>
+      <c r="G68" t="s">
+        <v>376</v>
+      </c>
+      <c r="J68" t="s">
+        <v>400</v>
+      </c>
+      <c r="K68" s="5">
+        <v>18535350</v>
+      </c>
+      <c r="L68" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300632/summary</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>300644</v>
+      </c>
+      <c r="B69" t="s">
+        <v>225</v>
+      </c>
+      <c r="D69" s="8">
+        <v>2019</v>
+      </c>
+      <c r="E69" s="8">
+        <v>2026</v>
+      </c>
+      <c r="F69" t="s">
+        <v>226</v>
+      </c>
+      <c r="G69" t="s">
+        <v>382</v>
+      </c>
+      <c r="J69" t="s">
+        <v>400</v>
+      </c>
+      <c r="K69" s="5">
+        <v>37800000</v>
+      </c>
+      <c r="L69" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300644/summary</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>300649</v>
+      </c>
+      <c r="B70" t="s">
+        <v>228</v>
+      </c>
+      <c r="D70" s="8">
+        <v>2019</v>
+      </c>
+      <c r="E70" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F70" t="s">
+        <v>229</v>
+      </c>
+      <c r="G70" t="s">
+        <v>361</v>
+      </c>
+      <c r="J70" t="s">
+        <v>400</v>
+      </c>
+      <c r="K70" s="5">
+        <v>25828000</v>
+      </c>
+      <c r="L70" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300649/summary</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>300654</v>
+      </c>
+      <c r="B71" t="s">
+        <v>231</v>
+      </c>
+      <c r="D71" s="8">
+        <v>2019</v>
+      </c>
+      <c r="E71" s="8">
+        <v>2025</v>
+      </c>
+      <c r="F71" t="s">
+        <v>232</v>
+      </c>
+      <c r="G71" t="s">
+        <v>384</v>
+      </c>
+      <c r="J71" t="s">
+        <v>400</v>
+      </c>
+      <c r="K71" s="5">
+        <v>12124941</v>
+      </c>
+      <c r="L71" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300654/summary</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>300655</v>
+      </c>
+      <c r="B72" t="s">
+        <v>234</v>
+      </c>
+      <c r="D72" s="8">
+        <v>2018</v>
+      </c>
+      <c r="E72" s="8">
+        <v>2026</v>
+      </c>
+      <c r="F72" t="s">
+        <v>235</v>
+      </c>
+      <c r="G72" t="s">
+        <v>385</v>
+      </c>
+      <c r="J72" t="s">
+        <v>400</v>
+      </c>
+      <c r="K72" s="5">
+        <v>20000000</v>
+      </c>
+      <c r="L72" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300655/summary</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>300656</v>
+      </c>
+      <c r="B73" t="s">
+        <v>237</v>
+      </c>
+      <c r="D73" s="8">
+        <v>2019</v>
+      </c>
+      <c r="E73" s="8">
+        <v>2024</v>
+      </c>
+      <c r="F73" t="s">
+        <v>238</v>
+      </c>
+      <c r="G73" t="s">
+        <v>347</v>
+      </c>
+      <c r="J73" t="s">
+        <v>400</v>
+      </c>
+      <c r="K73" s="5">
+        <v>12000000</v>
+      </c>
+      <c r="L73" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300656/summary</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>300708</v>
+      </c>
+      <c r="B74" t="s">
+        <v>243</v>
+      </c>
+      <c r="D74" s="8">
+        <v>2020</v>
+      </c>
+      <c r="E74" s="8">
+        <v>2026</v>
+      </c>
+      <c r="F74" t="s">
+        <v>244</v>
+      </c>
+      <c r="G74" t="s">
+        <v>347</v>
+      </c>
+      <c r="J74" t="s">
+        <v>400</v>
+      </c>
+      <c r="K74" s="5">
+        <v>49947720</v>
+      </c>
+      <c r="L74" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300708/summary</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>300755</v>
+      </c>
+      <c r="B75" t="s">
+        <v>249</v>
+      </c>
+      <c r="D75" s="8">
+        <v>2019</v>
+      </c>
+      <c r="E75" s="8">
+        <v>2024</v>
+      </c>
+      <c r="F75" t="s">
+        <v>250</v>
+      </c>
+      <c r="G75" t="s">
+        <v>387</v>
+      </c>
+      <c r="J75" t="s">
+        <v>400</v>
+      </c>
+      <c r="K75" s="5">
+        <v>16000000</v>
+      </c>
+      <c r="L75" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300755/summary</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>300760</v>
+      </c>
+      <c r="B76" t="s">
+        <v>252</v>
+      </c>
+      <c r="D76" s="8">
+        <v>2019</v>
+      </c>
+      <c r="E76" s="8">
+        <v>2026</v>
+      </c>
+      <c r="F76" t="s">
+        <v>253</v>
+      </c>
+      <c r="G76" t="s">
+        <v>347</v>
+      </c>
+      <c r="J76" t="s">
+        <v>400</v>
+      </c>
+      <c r="K76" s="5">
+        <v>35050000</v>
+      </c>
+      <c r="L76" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300760/summary</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>300781</v>
+      </c>
+      <c r="B77" t="s">
+        <v>257</v>
+      </c>
+      <c r="D77" s="8">
+        <v>2018</v>
+      </c>
+      <c r="E77" s="8">
+        <v>2025</v>
+      </c>
+      <c r="F77" t="s">
+        <v>258</v>
+      </c>
+      <c r="G77" t="s">
+        <v>377</v>
+      </c>
+      <c r="J77" t="s">
+        <v>400</v>
+      </c>
+      <c r="K77" s="5">
+        <v>20000000</v>
+      </c>
+      <c r="L77" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300781/summary</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>300785</v>
+      </c>
+      <c r="B78" t="s">
+        <v>261</v>
+      </c>
+      <c r="D78" s="8">
+        <v>2019</v>
+      </c>
+      <c r="E78" s="8">
+        <v>2024</v>
+      </c>
+      <c r="F78" t="s">
+        <v>262</v>
+      </c>
+      <c r="G78" t="s">
+        <v>390</v>
+      </c>
+      <c r="J78" t="s">
+        <v>400</v>
+      </c>
+      <c r="K78" s="5">
+        <v>4985058</v>
+      </c>
+      <c r="L78" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300785/summary</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>300815</v>
+      </c>
+      <c r="B79" t="s">
+        <v>264</v>
+      </c>
+      <c r="D79" s="8">
+        <v>2019</v>
+      </c>
+      <c r="E79" s="8">
+        <v>2024</v>
+      </c>
+      <c r="F79" t="s">
+        <v>265</v>
+      </c>
+      <c r="G79" t="s">
+        <v>347</v>
+      </c>
+      <c r="J79" t="s">
+        <v>400</v>
+      </c>
+      <c r="K79" s="5">
+        <v>19800000</v>
+      </c>
+      <c r="L79" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300815/summary</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>300849</v>
+      </c>
+      <c r="B80" t="s">
+        <v>267</v>
+      </c>
+      <c r="D80" s="8">
+        <v>2019</v>
+      </c>
+      <c r="E80" s="8">
+        <v>2024</v>
+      </c>
+      <c r="F80" t="s">
+        <v>268</v>
+      </c>
+      <c r="G80" t="s">
+        <v>348</v>
+      </c>
+      <c r="J80" t="s">
+        <v>400</v>
+      </c>
+      <c r="K80" s="5">
+        <v>4900000</v>
+      </c>
+      <c r="L80" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300849/summary</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>300966</v>
+      </c>
+      <c r="B81" t="s">
+        <v>270</v>
+      </c>
+      <c r="D81" s="8">
+        <v>2019</v>
+      </c>
+      <c r="E81" s="8">
+        <v>2025</v>
+      </c>
+      <c r="F81" t="s">
+        <v>271</v>
+      </c>
+      <c r="G81" t="s">
+        <v>347</v>
+      </c>
+      <c r="J81" t="s">
+        <v>400</v>
+      </c>
+      <c r="K81" s="5">
+        <v>19266871</v>
+      </c>
+      <c r="L81" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-300966/summary</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>301050</v>
+      </c>
+      <c r="B82" t="s">
+        <v>272</v>
+      </c>
+      <c r="D82" s="8">
+        <v>2022</v>
+      </c>
+      <c r="E82" s="8">
+        <v>2025</v>
+      </c>
+      <c r="F82" t="s">
+        <v>273</v>
+      </c>
+      <c r="G82" t="s">
+        <v>347</v>
+      </c>
+      <c r="J82" t="s">
+        <v>400</v>
+      </c>
+      <c r="K82" s="5">
+        <v>4700000</v>
+      </c>
+      <c r="L82" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-301050/summary</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>301067</v>
+      </c>
+      <c r="B83" t="s">
+        <v>274</v>
+      </c>
+      <c r="D83" s="8">
+        <v>2021</v>
+      </c>
+      <c r="E83" s="8">
+        <v>2025</v>
+      </c>
+      <c r="F83" t="s">
+        <v>275</v>
+      </c>
+      <c r="G83" t="s">
+        <v>347</v>
+      </c>
+      <c r="J83" t="s">
+        <v>400</v>
+      </c>
+      <c r="K83" s="5">
+        <v>32850000</v>
+      </c>
+      <c r="L83" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-301067/summary</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>301108</v>
+      </c>
+      <c r="B84" t="s">
+        <v>276</v>
+      </c>
+      <c r="D84" s="8">
+        <v>2020</v>
+      </c>
+      <c r="E84" s="8">
+        <v>2025</v>
+      </c>
+      <c r="F84" t="s">
+        <v>277</v>
+      </c>
+      <c r="G84" t="s">
+        <v>391</v>
+      </c>
+      <c r="J84" t="s">
+        <v>400</v>
+      </c>
+      <c r="K84" s="5">
+        <v>9400000</v>
+      </c>
+      <c r="L84" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-301108/summary</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>301132</v>
+      </c>
+      <c r="B85" t="s">
+        <v>280</v>
+      </c>
+      <c r="D85" s="8">
+        <v>2020</v>
+      </c>
+      <c r="E85" s="8">
+        <v>2026</v>
+      </c>
+      <c r="F85" t="s">
+        <v>281</v>
+      </c>
+      <c r="G85" t="s">
+        <v>397</v>
+      </c>
+      <c r="J85" t="s">
+        <v>400</v>
+      </c>
+      <c r="K85" s="5">
+        <v>7972870</v>
+      </c>
+      <c r="L85" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-301132/summary</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>301135</v>
+      </c>
+      <c r="B86" t="s">
+        <v>289</v>
+      </c>
+      <c r="D86" s="8">
+        <v>2020</v>
+      </c>
+      <c r="E86" s="8">
+        <v>2026</v>
+      </c>
+      <c r="F86" t="s">
+        <v>290</v>
+      </c>
+      <c r="G86" t="s">
+        <v>365</v>
+      </c>
+      <c r="J86" t="s">
+        <v>400</v>
+      </c>
+      <c r="K86" s="5">
+        <v>7953129</v>
+      </c>
+      <c r="L86" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-301135/summary</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>301136</v>
+      </c>
+      <c r="B87" t="s">
+        <v>292</v>
+      </c>
+      <c r="D87" s="8">
+        <v>2020</v>
+      </c>
+      <c r="E87" s="8">
+        <v>2026</v>
+      </c>
+      <c r="F87" t="s">
+        <v>293</v>
+      </c>
+      <c r="G87" t="s">
+        <v>396</v>
+      </c>
+      <c r="J87" t="s">
+        <v>400</v>
+      </c>
+      <c r="K87" s="5">
+        <v>8000000</v>
+      </c>
+      <c r="L87" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-301136/summary</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>301138</v>
+      </c>
+      <c r="B88" t="s">
+        <v>295</v>
+      </c>
+      <c r="D88" s="8">
+        <v>2020</v>
+      </c>
+      <c r="E88" s="8">
+        <v>2026</v>
+      </c>
+      <c r="F88" t="s">
+        <v>296</v>
+      </c>
+      <c r="G88" t="s">
+        <v>370</v>
+      </c>
+      <c r="J88" t="s">
+        <v>400</v>
+      </c>
+      <c r="K88" s="5">
+        <v>7903834</v>
+      </c>
+      <c r="L88" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-301138/summary</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>301139</v>
+      </c>
+      <c r="B89" t="s">
+        <v>298</v>
+      </c>
+      <c r="D89" s="8">
+        <v>2020</v>
+      </c>
+      <c r="E89" s="8">
+        <v>2026</v>
+      </c>
+      <c r="F89" t="s">
+        <v>299</v>
+      </c>
+      <c r="G89" t="s">
+        <v>398</v>
+      </c>
+      <c r="J89" t="s">
+        <v>400</v>
+      </c>
+      <c r="K89" s="5">
+        <v>7812831</v>
+      </c>
+      <c r="L89" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-301139/summary</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>301263</v>
+      </c>
+      <c r="B90" t="s">
+        <v>301</v>
+      </c>
+      <c r="D90" s="8">
+        <v>2021</v>
+      </c>
+      <c r="E90" s="8">
+        <v>2027</v>
+      </c>
+      <c r="F90" t="s">
+        <v>302</v>
+      </c>
+      <c r="G90" t="s">
+        <v>347</v>
+      </c>
+      <c r="J90" t="s">
+        <v>400</v>
+      </c>
+      <c r="K90" s="5">
+        <v>19000000</v>
+      </c>
+      <c r="L90" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-301263/summary</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>301290</v>
+      </c>
+      <c r="B91" t="s">
+        <v>304</v>
+      </c>
+      <c r="D91" s="8">
+        <v>2020</v>
+      </c>
+      <c r="E91" s="8">
+        <v>2024</v>
+      </c>
+      <c r="F91" t="s">
+        <v>305</v>
+      </c>
+      <c r="G91" t="s">
+        <v>347</v>
+      </c>
+      <c r="J91" t="s">
+        <v>400</v>
+      </c>
+      <c r="K91" s="5">
+        <v>4790000</v>
+      </c>
+      <c r="L91" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-301290/summary</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>301291</v>
+      </c>
+      <c r="B92" t="s">
+        <v>306</v>
+      </c>
+      <c r="D92" s="8">
+        <v>2020</v>
+      </c>
+      <c r="E92" s="8">
+        <v>2025</v>
+      </c>
+      <c r="F92" t="s">
+        <v>307</v>
+      </c>
+      <c r="G92" t="s">
+        <v>347</v>
+      </c>
+      <c r="J92" t="s">
+        <v>400</v>
+      </c>
+      <c r="K92" s="5">
+        <v>10739851</v>
+      </c>
+      <c r="L92" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://devtracker.fcdo.gov.uk/projects/GB-GOV-1-301291/summary</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Calibri"&amp;10&amp;K000000OFFICIAL&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>